<commit_message>
Added yolo, debugged posture model
</commit_message>
<xml_diff>
--- a/model/personalized_dataset.xlsx
+++ b/model/personalized_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1198,6 +1198,1051 @@
         <v>0</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>24.9816047538945</v>
+      </c>
+      <c r="B70" t="n">
+        <v>5.628583713734685</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>48.02857225639664</v>
+      </c>
+      <c r="B71" t="n">
+        <v>17.72820822527561</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>39.2797576724562</v>
+      </c>
+      <c r="B72" t="n">
+        <v>11.28711962152653</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>33.94633936788146</v>
+      </c>
+      <c r="B73" t="n">
+        <v>15.17141382329406</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>16.23978081344811</v>
+      </c>
+      <c r="B74" t="n">
+        <v>9.985844582977499</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>12.32334448672798</v>
+      </c>
+      <c r="B75" t="n">
+        <v>13.20765846071259</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>44.64704583099741</v>
+      </c>
+      <c r="B76" t="n">
+        <v>20.11102277086097</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>34.04460046972835</v>
+      </c>
+      <c r="B77" t="n">
+        <v>9.575963309832449</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>38.32290311184182</v>
+      </c>
+      <c r="B78" t="n">
+        <v>6.539598196575859</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>10.8233797718321</v>
+      </c>
+      <c r="B79" t="n">
+        <v>10.79502905827536</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>48.79639408647977</v>
+      </c>
+      <c r="B80" t="n">
+        <v>8.224425745080088</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>43.29770563201687</v>
+      </c>
+      <c r="B81" t="n">
+        <v>23.59395304685146</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>18.49356442713105</v>
+      </c>
+      <c r="B82" t="n">
+        <v>21.16240759128834</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>17.27299868828403</v>
+      </c>
+      <c r="B83" t="n">
+        <v>17.66807513020847</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>17.33618039413735</v>
+      </c>
+      <c r="B84" t="n">
+        <v>22.42921180375436</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>22.16968971838151</v>
+      </c>
+      <c r="B85" t="n">
+        <v>21.07344153798229</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30.99025726528951</v>
+      </c>
+      <c r="B86" t="n">
+        <v>8.731401177720716</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>27.27780074568463</v>
+      </c>
+      <c r="B87" t="n">
+        <v>22.85117996979956</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>21.64916560792168</v>
+      </c>
+      <c r="B88" t="n">
+        <v>15.78684483831301</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>34.47411578889518</v>
+      </c>
+      <c r="B89" t="n">
+        <v>21.14880310328125</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>15.57975442608167</v>
+      </c>
+      <c r="B90" t="n">
+        <v>22.92182599846986</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>21.68578594140872</v>
+      </c>
+      <c r="B91" t="n">
+        <v>11.36006949943728</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>24.65447373174767</v>
+      </c>
+      <c r="B92" t="n">
+        <v>7.201038490553535</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>28.24279936868144</v>
+      </c>
+      <c r="B93" t="n">
+        <v>9.558703250838834</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>17.98695128633439</v>
+      </c>
+      <c r="B94" t="n">
+        <v>21.36029531844986</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30.56937753654447</v>
+      </c>
+      <c r="B95" t="n">
+        <v>22.21461166512687</v>
+      </c>
+      <c r="C95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>33.6965827544817</v>
+      </c>
+      <c r="B96" t="n">
+        <v>5.139042610623815</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>11.85801650879991</v>
+      </c>
+      <c r="B97" t="n">
+        <v>15.21494605155132</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>34.30179407605753</v>
+      </c>
+      <c r="B98" t="n">
+        <v>13.34822006297558</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>16.82096494749166</v>
+      </c>
+      <c r="B99" t="n">
+        <v>9.442156209414605</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>12.60206371941118</v>
+      </c>
+      <c r="B100" t="n">
+        <v>7.397307346673657</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>48.62528132298237</v>
+      </c>
+      <c r="B101" t="n">
+        <v>23.85819407825038</v>
+      </c>
+      <c r="C101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>42.33589392465844</v>
+      </c>
+      <c r="B102" t="n">
+        <v>11.4640586404151</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>22.18455076693483</v>
+      </c>
+      <c r="B103" t="n">
+        <v>15.37581243486732</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>13.90688456025535</v>
+      </c>
+      <c r="B104" t="n">
+        <v>19.06037917790356</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>37.36932106048627</v>
+      </c>
+      <c r="B105" t="n">
+        <v>12.27259204758588</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>27.60609974958405</v>
+      </c>
+      <c r="B106" t="n">
+        <v>24.43564165441921</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>14.88152939379115</v>
+      </c>
+      <c r="B107" t="n">
+        <v>24.24894589884222</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>29.80707640445081</v>
+      </c>
+      <c r="B108" t="n">
+        <v>10.03564591650728</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>11.37554084460874</v>
+      </c>
+      <c r="B109" t="n">
+        <v>14.94497011784771</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>46.37281608315129</v>
+      </c>
+      <c r="B110" t="n">
+        <v>11.01756619633539</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>20.35119926400068</v>
+      </c>
+      <c r="B111" t="n">
+        <v>10.69680988754935</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>36.50089137415928</v>
+      </c>
+      <c r="B112" t="n">
+        <v>5.737738947090656</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>22.46844304357644</v>
+      </c>
+      <c r="B113" t="n">
+        <v>17.19128667959794</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>30.80272084711243</v>
+      </c>
+      <c r="B114" t="n">
+        <v>15.05358046457723</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>31.86841117373119</v>
+      </c>
+      <c r="B115" t="n">
+        <v>6.029575024999787</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>17.39417822102108</v>
+      </c>
+      <c r="B116" t="n">
+        <v>10.57292928473223</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>48.78338511058234</v>
+      </c>
+      <c r="B117" t="n">
+        <v>23.16531771933307</v>
+      </c>
+      <c r="C117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>41.00531293444458</v>
+      </c>
+      <c r="B118" t="n">
+        <v>9.791237813339448</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>47.57995766256757</v>
+      </c>
+      <c r="B119" t="n">
+        <v>7.897897441824462</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>45.79309401710595</v>
+      </c>
+      <c r="B120" t="n">
+        <v>14.78905520555126</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>33.9159991524434</v>
+      </c>
+      <c r="B121" t="n">
+        <v>24.71300908221201</v>
+      </c>
+      <c r="C121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>46.87496940092467</v>
+      </c>
+      <c r="B122" t="n">
+        <v>9.841105430230009</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>13.53970008207678</v>
+      </c>
+      <c r="B123" t="n">
+        <v>18.44271094811757</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>17.83931449676581</v>
+      </c>
+      <c r="B124" t="n">
+        <v>20.23239230657435</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>11.80909155642152</v>
+      </c>
+      <c r="B125" t="n">
+        <v>9.752750879847994</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>23.01321323053057</v>
+      </c>
+      <c r="B126" t="n">
+        <v>19.56432697223719</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>25.54709158757928</v>
+      </c>
+      <c r="B127" t="n">
+        <v>12.35566265438506</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>20.85396127095584</v>
+      </c>
+      <c r="B128" t="n">
+        <v>17.64611661187159</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>43.14950036607718</v>
+      </c>
+      <c r="B129" t="n">
+        <v>17.6705942152179</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>24.27013306774357</v>
+      </c>
+      <c r="B130" t="n">
+        <v>15.71549368149517</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>21.23738038749523</v>
+      </c>
+      <c r="B131" t="n">
+        <v>6.805795401088166</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>31.70784332632994</v>
+      </c>
+      <c r="B132" t="n">
+        <v>21.70604991178476</v>
+      </c>
+      <c r="C132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>15.63696899899051</v>
+      </c>
+      <c r="B133" t="n">
+        <v>11.41560129943472</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>42.08787923016159</v>
+      </c>
+      <c r="B134" t="n">
+        <v>8.730370207997085</v>
+      </c>
+      <c r="C134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>12.98202574719083</v>
+      </c>
+      <c r="B135" t="n">
+        <v>5.815502831095278</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>49.47547746402069</v>
+      </c>
+      <c r="B136" t="n">
+        <v>16.81785886376484</v>
+      </c>
+      <c r="C136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>40.88979077186629</v>
+      </c>
+      <c r="B137" t="n">
+        <v>18.55128723684565</v>
+      </c>
+      <c r="C137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>17.94862726136689</v>
+      </c>
+      <c r="B138" t="n">
+        <v>5.331756578557123</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>10.2208846849441</v>
+      </c>
+      <c r="B139" t="n">
+        <v>15.24186116598562</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>42.61845713819336</v>
+      </c>
+      <c r="B140" t="n">
+        <v>9.529915503958758</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>38.27429375390469</v>
+      </c>
+      <c r="B141" t="n">
+        <v>17.903455808189</v>
+      </c>
+      <c r="C141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>39.16028672163949</v>
+      </c>
+      <c r="B142" t="n">
+        <v>8.487328580099829</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>40.85081386743783</v>
+      </c>
+      <c r="B143" t="n">
+        <v>18.81875476204932</v>
+      </c>
+      <c r="C143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>12.96178606936362</v>
+      </c>
+      <c r="B144" t="n">
+        <v>12.73470692601075</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>24.33862914177091</v>
+      </c>
+      <c r="B145" t="n">
+        <v>23.73459977473469</v>
+      </c>
+      <c r="C145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>14.63476238100519</v>
+      </c>
+      <c r="B146" t="n">
+        <v>7.750418882919865</v>
+      </c>
+      <c r="C146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>44.52413703502374</v>
+      </c>
+      <c r="B147" t="n">
+        <v>11.82132702100517</v>
+      </c>
+      <c r="C147" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>34.93192507310232</v>
+      </c>
+      <c r="B148" t="n">
+        <v>7.269470424811781</v>
+      </c>
+      <c r="C148" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>23.23592099410597</v>
+      </c>
+      <c r="B149" t="n">
+        <v>23.49387236557126</v>
+      </c>
+      <c r="C149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>12.54233401144095</v>
+      </c>
+      <c r="B150" t="n">
+        <v>22.54678706761962</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>22.43929286862649</v>
+      </c>
+      <c r="B151" t="n">
+        <v>10.15883255430311</v>
+      </c>
+      <c r="C151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>23.00733288106988</v>
+      </c>
+      <c r="B152" t="n">
+        <v>18.19968092068358</v>
+      </c>
+      <c r="C152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>39.18424713352256</v>
+      </c>
+      <c r="B153" t="n">
+        <v>21.34444400402432</v>
+      </c>
+      <c r="C153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>35.50229885420853</v>
+      </c>
+      <c r="B154" t="n">
+        <v>16.10401623198925</v>
+      </c>
+      <c r="C154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>45.48850970305306</v>
+      </c>
+      <c r="B155" t="n">
+        <v>15.59301156712013</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>28.88859700647797</v>
+      </c>
+      <c r="B156" t="n">
+        <v>9.837045818009035</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>14.78376983753207</v>
+      </c>
+      <c r="B157" t="n">
+        <v>6.862055356117985</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>38.5297914889198</v>
+      </c>
+      <c r="B158" t="n">
+        <v>22.94431515906653</v>
+      </c>
+      <c r="C158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>40.4314019446759</v>
+      </c>
+      <c r="B159" t="n">
+        <v>23.00836114326661</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>40.83868719818244</v>
+      </c>
+      <c r="B160" t="n">
+        <v>11.78059582097401</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>29.75182385457563</v>
+      </c>
+      <c r="B161" t="n">
+        <v>11.98419149225322</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>27.10164073434198</v>
+      </c>
+      <c r="B162" t="n">
+        <v>22.94220519905154</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>11.01676506976381</v>
+      </c>
+      <c r="B163" t="n">
+        <v>22.74172848530235</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>14.31565707973218</v>
+      </c>
+      <c r="B164" t="n">
+        <v>20.59751091715248</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
yolo threading sensing integration
</commit_message>
<xml_diff>
--- a/model/personalized_dataset.xlsx
+++ b/model/personalized_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:C360"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2243,6 +2243,2162 @@
         <v>0</v>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>24.9816047538945</v>
+      </c>
+      <c r="B165" t="n">
+        <v>5.628583713734685</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>48.02857225639664</v>
+      </c>
+      <c r="B166" t="n">
+        <v>17.72820822527561</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>39.2797576724562</v>
+      </c>
+      <c r="B167" t="n">
+        <v>11.28711962152653</v>
+      </c>
+      <c r="C167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>33.94633936788146</v>
+      </c>
+      <c r="B168" t="n">
+        <v>15.17141382329406</v>
+      </c>
+      <c r="C168" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>16.24074561769746</v>
+      </c>
+      <c r="B169" t="n">
+        <v>23.15132947852186</v>
+      </c>
+      <c r="C169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>16.23978081344811</v>
+      </c>
+      <c r="B170" t="n">
+        <v>9.985844582977499</v>
+      </c>
+      <c r="C170" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>12.32334448672798</v>
+      </c>
+      <c r="B171" t="n">
+        <v>13.20765846071259</v>
+      </c>
+      <c r="C171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>44.64704583099741</v>
+      </c>
+      <c r="B172" t="n">
+        <v>20.11102277086097</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>34.04460046972835</v>
+      </c>
+      <c r="B173" t="n">
+        <v>9.575963309832449</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>38.32290311184182</v>
+      </c>
+      <c r="B174" t="n">
+        <v>6.539598196575859</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>10.8233797718321</v>
+      </c>
+      <c r="B175" t="n">
+        <v>10.79502905827536</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>48.79639408647977</v>
+      </c>
+      <c r="B176" t="n">
+        <v>8.224425745080088</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>43.29770563201687</v>
+      </c>
+      <c r="B177" t="n">
+        <v>23.59395304685146</v>
+      </c>
+      <c r="C177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>18.49356442713105</v>
+      </c>
+      <c r="B178" t="n">
+        <v>21.16240759128834</v>
+      </c>
+      <c r="C178" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>17.27299868828403</v>
+      </c>
+      <c r="B179" t="n">
+        <v>17.66807513020847</v>
+      </c>
+      <c r="C179" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>17.33618039413735</v>
+      </c>
+      <c r="B180" t="n">
+        <v>22.42921180375436</v>
+      </c>
+      <c r="C180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>22.16968971838151</v>
+      </c>
+      <c r="B181" t="n">
+        <v>21.07344153798229</v>
+      </c>
+      <c r="C181" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>30.99025726528951</v>
+      </c>
+      <c r="B182" t="n">
+        <v>8.731401177720716</v>
+      </c>
+      <c r="C182" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>27.27780074568463</v>
+      </c>
+      <c r="B183" t="n">
+        <v>22.85117996979956</v>
+      </c>
+      <c r="C183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>21.64916560792168</v>
+      </c>
+      <c r="B184" t="n">
+        <v>15.78684483831301</v>
+      </c>
+      <c r="C184" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>34.47411578889518</v>
+      </c>
+      <c r="B185" t="n">
+        <v>21.14880310328125</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>15.57975442608167</v>
+      </c>
+      <c r="B186" t="n">
+        <v>22.92182599846986</v>
+      </c>
+      <c r="C186" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>21.68578594140872</v>
+      </c>
+      <c r="B187" t="n">
+        <v>11.36006949943728</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>24.65447373174767</v>
+      </c>
+      <c r="B188" t="n">
+        <v>7.201038490553535</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>28.24279936868144</v>
+      </c>
+      <c r="B189" t="n">
+        <v>9.558703250838834</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>41.40703845572055</v>
+      </c>
+      <c r="B190" t="n">
+        <v>13.54215577252513</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>17.98695128633439</v>
+      </c>
+      <c r="B191" t="n">
+        <v>21.36029531844986</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>30.56937753654447</v>
+      </c>
+      <c r="B192" t="n">
+        <v>22.21461166512687</v>
+      </c>
+      <c r="C192" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>33.6965827544817</v>
+      </c>
+      <c r="B193" t="n">
+        <v>5.139042610623815</v>
+      </c>
+      <c r="C193" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>11.85801650879991</v>
+      </c>
+      <c r="B194" t="n">
+        <v>15.21494605155132</v>
+      </c>
+      <c r="C194" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>34.30179407605753</v>
+      </c>
+      <c r="B195" t="n">
+        <v>13.34822006297558</v>
+      </c>
+      <c r="C195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>16.82096494749166</v>
+      </c>
+      <c r="B196" t="n">
+        <v>9.442156209414605</v>
+      </c>
+      <c r="C196" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>12.60206371941118</v>
+      </c>
+      <c r="B197" t="n">
+        <v>7.397307346673657</v>
+      </c>
+      <c r="C197" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>48.62528132298237</v>
+      </c>
+      <c r="B198" t="n">
+        <v>23.85819407825038</v>
+      </c>
+      <c r="C198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>42.33589392465844</v>
+      </c>
+      <c r="B199" t="n">
+        <v>11.4640586404151</v>
+      </c>
+      <c r="C199" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>22.18455076693483</v>
+      </c>
+      <c r="B200" t="n">
+        <v>15.37581243486732</v>
+      </c>
+      <c r="C200" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>13.90688456025535</v>
+      </c>
+      <c r="B201" t="n">
+        <v>19.06037917790356</v>
+      </c>
+      <c r="C201" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>37.36932106048627</v>
+      </c>
+      <c r="B202" t="n">
+        <v>12.27259204758588</v>
+      </c>
+      <c r="C202" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>27.60609974958405</v>
+      </c>
+      <c r="B203" t="n">
+        <v>24.43564165441921</v>
+      </c>
+      <c r="C203" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>14.88152939379115</v>
+      </c>
+      <c r="B204" t="n">
+        <v>24.24894589884222</v>
+      </c>
+      <c r="C204" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>29.80707640445081</v>
+      </c>
+      <c r="B205" t="n">
+        <v>10.03564591650728</v>
+      </c>
+      <c r="C205" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>11.37554084460874</v>
+      </c>
+      <c r="B206" t="n">
+        <v>14.94497011784771</v>
+      </c>
+      <c r="C206" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>46.37281608315129</v>
+      </c>
+      <c r="B207" t="n">
+        <v>11.01756619633539</v>
+      </c>
+      <c r="C207" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>20.35119926400068</v>
+      </c>
+      <c r="B208" t="n">
+        <v>10.69680988754935</v>
+      </c>
+      <c r="C208" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>36.50089137415928</v>
+      </c>
+      <c r="B209" t="n">
+        <v>5.737738947090656</v>
+      </c>
+      <c r="C209" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>22.46844304357644</v>
+      </c>
+      <c r="B210" t="n">
+        <v>17.19128667959794</v>
+      </c>
+      <c r="C210" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>30.80272084711243</v>
+      </c>
+      <c r="B211" t="n">
+        <v>15.05358046457723</v>
+      </c>
+      <c r="C211" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>31.86841117373119</v>
+      </c>
+      <c r="B212" t="n">
+        <v>6.029575024999787</v>
+      </c>
+      <c r="C212" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>17.39417822102108</v>
+      </c>
+      <c r="B213" t="n">
+        <v>10.57292928473223</v>
+      </c>
+      <c r="C213" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>48.78338511058234</v>
+      </c>
+      <c r="B214" t="n">
+        <v>23.16531771933307</v>
+      </c>
+      <c r="C214" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>41.00531293444458</v>
+      </c>
+      <c r="B215" t="n">
+        <v>9.791237813339448</v>
+      </c>
+      <c r="C215" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>47.57995766256757</v>
+      </c>
+      <c r="B216" t="n">
+        <v>7.897897441824462</v>
+      </c>
+      <c r="C216" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>45.79309401710595</v>
+      </c>
+      <c r="B217" t="n">
+        <v>14.78905520555126</v>
+      </c>
+      <c r="C217" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>33.9159991524434</v>
+      </c>
+      <c r="B218" t="n">
+        <v>24.71300908221201</v>
+      </c>
+      <c r="C218" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>46.87496940092467</v>
+      </c>
+      <c r="B219" t="n">
+        <v>9.841105430230009</v>
+      </c>
+      <c r="C219" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>13.53970008207678</v>
+      </c>
+      <c r="B220" t="n">
+        <v>18.44271094811757</v>
+      </c>
+      <c r="C220" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>17.83931449676581</v>
+      </c>
+      <c r="B221" t="n">
+        <v>20.23239230657435</v>
+      </c>
+      <c r="C221" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>11.80909155642152</v>
+      </c>
+      <c r="B222" t="n">
+        <v>9.752750879847994</v>
+      </c>
+      <c r="C222" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>23.01321323053057</v>
+      </c>
+      <c r="B223" t="n">
+        <v>19.56432697223719</v>
+      </c>
+      <c r="C223" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>25.54709158757928</v>
+      </c>
+      <c r="B224" t="n">
+        <v>12.35566265438506</v>
+      </c>
+      <c r="C224" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>20.85396127095584</v>
+      </c>
+      <c r="B225" t="n">
+        <v>17.64611661187159</v>
+      </c>
+      <c r="C225" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>43.14950036607718</v>
+      </c>
+      <c r="B226" t="n">
+        <v>17.6705942152179</v>
+      </c>
+      <c r="C226" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>24.27013306774357</v>
+      </c>
+      <c r="B227" t="n">
+        <v>15.71549368149517</v>
+      </c>
+      <c r="C227" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>21.23738038749523</v>
+      </c>
+      <c r="B228" t="n">
+        <v>6.805795401088166</v>
+      </c>
+      <c r="C228" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>31.70784332632994</v>
+      </c>
+      <c r="B229" t="n">
+        <v>21.70604991178476</v>
+      </c>
+      <c r="C229" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>15.63696899899051</v>
+      </c>
+      <c r="B230" t="n">
+        <v>11.41560129943472</v>
+      </c>
+      <c r="C230" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>42.08787923016159</v>
+      </c>
+      <c r="B231" t="n">
+        <v>8.730370207997085</v>
+      </c>
+      <c r="C231" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>12.98202574719083</v>
+      </c>
+      <c r="B232" t="n">
+        <v>5.815502831095278</v>
+      </c>
+      <c r="C232" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>49.47547746402069</v>
+      </c>
+      <c r="B233" t="n">
+        <v>16.81785886376484</v>
+      </c>
+      <c r="C233" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>40.88979077186629</v>
+      </c>
+      <c r="B234" t="n">
+        <v>18.55128723684565</v>
+      </c>
+      <c r="C234" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>17.94862726136689</v>
+      </c>
+      <c r="B235" t="n">
+        <v>5.331756578557123</v>
+      </c>
+      <c r="C235" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>10.2208846849441</v>
+      </c>
+      <c r="B236" t="n">
+        <v>15.24186116598562</v>
+      </c>
+      <c r="C236" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>42.61845713819336</v>
+      </c>
+      <c r="B237" t="n">
+        <v>9.529915503958758</v>
+      </c>
+      <c r="C237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>38.27429375390469</v>
+      </c>
+      <c r="B238" t="n">
+        <v>17.903455808189</v>
+      </c>
+      <c r="C238" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>39.16028672163949</v>
+      </c>
+      <c r="B239" t="n">
+        <v>8.487328580099829</v>
+      </c>
+      <c r="C239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>40.85081386743783</v>
+      </c>
+      <c r="B240" t="n">
+        <v>18.81875476204932</v>
+      </c>
+      <c r="C240" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>12.96178606936362</v>
+      </c>
+      <c r="B241" t="n">
+        <v>12.73470692601075</v>
+      </c>
+      <c r="C241" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>24.33862914177091</v>
+      </c>
+      <c r="B242" t="n">
+        <v>23.73459977473469</v>
+      </c>
+      <c r="C242" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>14.63476238100519</v>
+      </c>
+      <c r="B243" t="n">
+        <v>7.750418882919865</v>
+      </c>
+      <c r="C243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>44.52413703502374</v>
+      </c>
+      <c r="B244" t="n">
+        <v>11.82132702100517</v>
+      </c>
+      <c r="C244" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>34.93192507310232</v>
+      </c>
+      <c r="B245" t="n">
+        <v>7.269470424811781</v>
+      </c>
+      <c r="C245" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>23.23592099410597</v>
+      </c>
+      <c r="B246" t="n">
+        <v>23.49387236557126</v>
+      </c>
+      <c r="C246" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>12.54233401144095</v>
+      </c>
+      <c r="B247" t="n">
+        <v>22.54678706761962</v>
+      </c>
+      <c r="C247" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>22.43929286862649</v>
+      </c>
+      <c r="B248" t="n">
+        <v>10.15883255430311</v>
+      </c>
+      <c r="C248" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>23.00733288106988</v>
+      </c>
+      <c r="B249" t="n">
+        <v>18.19968092068358</v>
+      </c>
+      <c r="C249" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>39.18424713352256</v>
+      </c>
+      <c r="B250" t="n">
+        <v>21.34444400402432</v>
+      </c>
+      <c r="C250" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>35.50229885420853</v>
+      </c>
+      <c r="B251" t="n">
+        <v>16.10401623198925</v>
+      </c>
+      <c r="C251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>45.48850970305306</v>
+      </c>
+      <c r="B252" t="n">
+        <v>15.59301156712013</v>
+      </c>
+      <c r="C252" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>28.88859700647797</v>
+      </c>
+      <c r="B253" t="n">
+        <v>9.837045818009035</v>
+      </c>
+      <c r="C253" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>14.78376983753207</v>
+      </c>
+      <c r="B254" t="n">
+        <v>6.862055356117985</v>
+      </c>
+      <c r="C254" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>38.5297914889198</v>
+      </c>
+      <c r="B255" t="n">
+        <v>22.94431515906653</v>
+      </c>
+      <c r="C255" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>40.4314019446759</v>
+      </c>
+      <c r="B256" t="n">
+        <v>23.00836114326661</v>
+      </c>
+      <c r="C256" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>32.45108790277985</v>
+      </c>
+      <c r="B257" t="n">
+        <v>17.66202914546536</v>
+      </c>
+      <c r="C257" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>40.83868719818244</v>
+      </c>
+      <c r="B258" t="n">
+        <v>11.78059582097401</v>
+      </c>
+      <c r="C258" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>29.75182385457563</v>
+      </c>
+      <c r="B259" t="n">
+        <v>11.98419149225322</v>
+      </c>
+      <c r="C259" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>27.10164073434198</v>
+      </c>
+      <c r="B260" t="n">
+        <v>22.94220519905154</v>
+      </c>
+      <c r="C260" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>11.01676506976381</v>
+      </c>
+      <c r="B261" t="n">
+        <v>22.74172848530235</v>
+      </c>
+      <c r="C261" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>14.31565707973218</v>
+      </c>
+      <c r="B262" t="n">
+        <v>20.59751091715248</v>
+      </c>
+      <c r="C262" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>24.9816047538945</v>
+      </c>
+      <c r="B263" t="n">
+        <v>5.628583713734685</v>
+      </c>
+      <c r="C263" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>48.02857225639664</v>
+      </c>
+      <c r="B264" t="n">
+        <v>17.72820822527561</v>
+      </c>
+      <c r="C264" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>39.2797576724562</v>
+      </c>
+      <c r="B265" t="n">
+        <v>11.28711962152653</v>
+      </c>
+      <c r="C265" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>33.94633936788146</v>
+      </c>
+      <c r="B266" t="n">
+        <v>15.17141382329406</v>
+      </c>
+      <c r="C266" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>16.24074561769746</v>
+      </c>
+      <c r="B267" t="n">
+        <v>23.15132947852186</v>
+      </c>
+      <c r="C267" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>16.23978081344811</v>
+      </c>
+      <c r="B268" t="n">
+        <v>9.985844582977499</v>
+      </c>
+      <c r="C268" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>12.32334448672798</v>
+      </c>
+      <c r="B269" t="n">
+        <v>13.20765846071259</v>
+      </c>
+      <c r="C269" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>44.64704583099741</v>
+      </c>
+      <c r="B270" t="n">
+        <v>20.11102277086097</v>
+      </c>
+      <c r="C270" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>34.04460046972835</v>
+      </c>
+      <c r="B271" t="n">
+        <v>9.575963309832449</v>
+      </c>
+      <c r="C271" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>38.32290311184182</v>
+      </c>
+      <c r="B272" t="n">
+        <v>6.539598196575859</v>
+      </c>
+      <c r="C272" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>10.8233797718321</v>
+      </c>
+      <c r="B273" t="n">
+        <v>10.79502905827536</v>
+      </c>
+      <c r="C273" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>48.79639408647977</v>
+      </c>
+      <c r="B274" t="n">
+        <v>8.224425745080088</v>
+      </c>
+      <c r="C274" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>43.29770563201687</v>
+      </c>
+      <c r="B275" t="n">
+        <v>23.59395304685146</v>
+      </c>
+      <c r="C275" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>18.49356442713105</v>
+      </c>
+      <c r="B276" t="n">
+        <v>21.16240759128834</v>
+      </c>
+      <c r="C276" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>17.27299868828403</v>
+      </c>
+      <c r="B277" t="n">
+        <v>17.66807513020847</v>
+      </c>
+      <c r="C277" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>17.33618039413735</v>
+      </c>
+      <c r="B278" t="n">
+        <v>22.42921180375436</v>
+      </c>
+      <c r="C278" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>22.16968971838151</v>
+      </c>
+      <c r="B279" t="n">
+        <v>21.07344153798229</v>
+      </c>
+      <c r="C279" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>30.99025726528951</v>
+      </c>
+      <c r="B280" t="n">
+        <v>8.731401177720716</v>
+      </c>
+      <c r="C280" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>27.27780074568463</v>
+      </c>
+      <c r="B281" t="n">
+        <v>22.85117996979956</v>
+      </c>
+      <c r="C281" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>21.64916560792168</v>
+      </c>
+      <c r="B282" t="n">
+        <v>15.78684483831301</v>
+      </c>
+      <c r="C282" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>34.47411578889518</v>
+      </c>
+      <c r="B283" t="n">
+        <v>21.14880310328125</v>
+      </c>
+      <c r="C283" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>15.57975442608167</v>
+      </c>
+      <c r="B284" t="n">
+        <v>22.92182599846986</v>
+      </c>
+      <c r="C284" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>21.68578594140872</v>
+      </c>
+      <c r="B285" t="n">
+        <v>11.36006949943728</v>
+      </c>
+      <c r="C285" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>24.65447373174767</v>
+      </c>
+      <c r="B286" t="n">
+        <v>7.201038490553535</v>
+      </c>
+      <c r="C286" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>28.24279936868144</v>
+      </c>
+      <c r="B287" t="n">
+        <v>9.558703250838834</v>
+      </c>
+      <c r="C287" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>41.40703845572055</v>
+      </c>
+      <c r="B288" t="n">
+        <v>13.54215577252513</v>
+      </c>
+      <c r="C288" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>17.98695128633439</v>
+      </c>
+      <c r="B289" t="n">
+        <v>21.36029531844986</v>
+      </c>
+      <c r="C289" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>30.56937753654447</v>
+      </c>
+      <c r="B290" t="n">
+        <v>22.21461166512687</v>
+      </c>
+      <c r="C290" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>33.6965827544817</v>
+      </c>
+      <c r="B291" t="n">
+        <v>5.139042610623815</v>
+      </c>
+      <c r="C291" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>11.85801650879991</v>
+      </c>
+      <c r="B292" t="n">
+        <v>15.21494605155132</v>
+      </c>
+      <c r="C292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>34.30179407605753</v>
+      </c>
+      <c r="B293" t="n">
+        <v>13.34822006297558</v>
+      </c>
+      <c r="C293" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>16.82096494749166</v>
+      </c>
+      <c r="B294" t="n">
+        <v>9.442156209414605</v>
+      </c>
+      <c r="C294" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>12.60206371941118</v>
+      </c>
+      <c r="B295" t="n">
+        <v>7.397307346673657</v>
+      </c>
+      <c r="C295" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>48.62528132298237</v>
+      </c>
+      <c r="B296" t="n">
+        <v>23.85819407825038</v>
+      </c>
+      <c r="C296" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>42.33589392465844</v>
+      </c>
+      <c r="B297" t="n">
+        <v>11.4640586404151</v>
+      </c>
+      <c r="C297" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>22.18455076693483</v>
+      </c>
+      <c r="B298" t="n">
+        <v>15.37581243486732</v>
+      </c>
+      <c r="C298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>13.90688456025535</v>
+      </c>
+      <c r="B299" t="n">
+        <v>19.06037917790356</v>
+      </c>
+      <c r="C299" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>37.36932106048627</v>
+      </c>
+      <c r="B300" t="n">
+        <v>12.27259204758588</v>
+      </c>
+      <c r="C300" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>27.60609974958405</v>
+      </c>
+      <c r="B301" t="n">
+        <v>24.43564165441921</v>
+      </c>
+      <c r="C301" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>14.88152939379115</v>
+      </c>
+      <c r="B302" t="n">
+        <v>24.24894589884222</v>
+      </c>
+      <c r="C302" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>29.80707640445081</v>
+      </c>
+      <c r="B303" t="n">
+        <v>10.03564591650728</v>
+      </c>
+      <c r="C303" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>11.37554084460874</v>
+      </c>
+      <c r="B304" t="n">
+        <v>14.94497011784771</v>
+      </c>
+      <c r="C304" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>46.37281608315129</v>
+      </c>
+      <c r="B305" t="n">
+        <v>11.01756619633539</v>
+      </c>
+      <c r="C305" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>20.35119926400068</v>
+      </c>
+      <c r="B306" t="n">
+        <v>10.69680988754935</v>
+      </c>
+      <c r="C306" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>36.50089137415928</v>
+      </c>
+      <c r="B307" t="n">
+        <v>5.737738947090656</v>
+      </c>
+      <c r="C307" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>22.46844304357644</v>
+      </c>
+      <c r="B308" t="n">
+        <v>17.19128667959794</v>
+      </c>
+      <c r="C308" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>30.80272084711243</v>
+      </c>
+      <c r="B309" t="n">
+        <v>15.05358046457723</v>
+      </c>
+      <c r="C309" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>31.86841117373119</v>
+      </c>
+      <c r="B310" t="n">
+        <v>6.029575024999787</v>
+      </c>
+      <c r="C310" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>17.39417822102108</v>
+      </c>
+      <c r="B311" t="n">
+        <v>10.57292928473223</v>
+      </c>
+      <c r="C311" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>48.78338511058234</v>
+      </c>
+      <c r="B312" t="n">
+        <v>23.16531771933307</v>
+      </c>
+      <c r="C312" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>41.00531293444458</v>
+      </c>
+      <c r="B313" t="n">
+        <v>9.791237813339448</v>
+      </c>
+      <c r="C313" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>47.57995766256757</v>
+      </c>
+      <c r="B314" t="n">
+        <v>7.897897441824462</v>
+      </c>
+      <c r="C314" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>45.79309401710595</v>
+      </c>
+      <c r="B315" t="n">
+        <v>14.78905520555126</v>
+      </c>
+      <c r="C315" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>33.9159991524434</v>
+      </c>
+      <c r="B316" t="n">
+        <v>24.71300908221201</v>
+      </c>
+      <c r="C316" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>46.87496940092467</v>
+      </c>
+      <c r="B317" t="n">
+        <v>9.841105430230009</v>
+      </c>
+      <c r="C317" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>13.53970008207678</v>
+      </c>
+      <c r="B318" t="n">
+        <v>18.44271094811757</v>
+      </c>
+      <c r="C318" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>17.83931449676581</v>
+      </c>
+      <c r="B319" t="n">
+        <v>20.23239230657435</v>
+      </c>
+      <c r="C319" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>11.80909155642152</v>
+      </c>
+      <c r="B320" t="n">
+        <v>9.752750879847994</v>
+      </c>
+      <c r="C320" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>23.01321323053057</v>
+      </c>
+      <c r="B321" t="n">
+        <v>19.56432697223719</v>
+      </c>
+      <c r="C321" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>25.54709158757928</v>
+      </c>
+      <c r="B322" t="n">
+        <v>12.35566265438506</v>
+      </c>
+      <c r="C322" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>20.85396127095584</v>
+      </c>
+      <c r="B323" t="n">
+        <v>17.64611661187159</v>
+      </c>
+      <c r="C323" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>43.14950036607718</v>
+      </c>
+      <c r="B324" t="n">
+        <v>17.6705942152179</v>
+      </c>
+      <c r="C324" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>24.27013306774357</v>
+      </c>
+      <c r="B325" t="n">
+        <v>15.71549368149517</v>
+      </c>
+      <c r="C325" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>21.23738038749523</v>
+      </c>
+      <c r="B326" t="n">
+        <v>6.805795401088166</v>
+      </c>
+      <c r="C326" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>31.70784332632994</v>
+      </c>
+      <c r="B327" t="n">
+        <v>21.70604991178476</v>
+      </c>
+      <c r="C327" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>15.63696899899051</v>
+      </c>
+      <c r="B328" t="n">
+        <v>11.41560129943472</v>
+      </c>
+      <c r="C328" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>42.08787923016159</v>
+      </c>
+      <c r="B329" t="n">
+        <v>8.730370207997085</v>
+      </c>
+      <c r="C329" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>12.98202574719083</v>
+      </c>
+      <c r="B330" t="n">
+        <v>5.815502831095278</v>
+      </c>
+      <c r="C330" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>49.47547746402069</v>
+      </c>
+      <c r="B331" t="n">
+        <v>16.81785886376484</v>
+      </c>
+      <c r="C331" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>40.88979077186629</v>
+      </c>
+      <c r="B332" t="n">
+        <v>18.55128723684565</v>
+      </c>
+      <c r="C332" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>17.94862726136689</v>
+      </c>
+      <c r="B333" t="n">
+        <v>5.331756578557123</v>
+      </c>
+      <c r="C333" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>10.2208846849441</v>
+      </c>
+      <c r="B334" t="n">
+        <v>15.24186116598562</v>
+      </c>
+      <c r="C334" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>42.61845713819336</v>
+      </c>
+      <c r="B335" t="n">
+        <v>9.529915503958758</v>
+      </c>
+      <c r="C335" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>38.27429375390469</v>
+      </c>
+      <c r="B336" t="n">
+        <v>17.903455808189</v>
+      </c>
+      <c r="C336" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>39.16028672163949</v>
+      </c>
+      <c r="B337" t="n">
+        <v>8.487328580099829</v>
+      </c>
+      <c r="C337" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>40.85081386743783</v>
+      </c>
+      <c r="B338" t="n">
+        <v>18.81875476204932</v>
+      </c>
+      <c r="C338" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>12.96178606936362</v>
+      </c>
+      <c r="B339" t="n">
+        <v>12.73470692601075</v>
+      </c>
+      <c r="C339" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>24.33862914177091</v>
+      </c>
+      <c r="B340" t="n">
+        <v>23.73459977473469</v>
+      </c>
+      <c r="C340" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>14.63476238100519</v>
+      </c>
+      <c r="B341" t="n">
+        <v>7.750418882919865</v>
+      </c>
+      <c r="C341" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>44.52413703502374</v>
+      </c>
+      <c r="B342" t="n">
+        <v>11.82132702100517</v>
+      </c>
+      <c r="C342" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>34.93192507310232</v>
+      </c>
+      <c r="B343" t="n">
+        <v>7.269470424811781</v>
+      </c>
+      <c r="C343" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>23.23592099410597</v>
+      </c>
+      <c r="B344" t="n">
+        <v>23.49387236557126</v>
+      </c>
+      <c r="C344" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>12.54233401144095</v>
+      </c>
+      <c r="B345" t="n">
+        <v>22.54678706761962</v>
+      </c>
+      <c r="C345" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>22.43929286862649</v>
+      </c>
+      <c r="B346" t="n">
+        <v>10.15883255430311</v>
+      </c>
+      <c r="C346" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>23.00733288106988</v>
+      </c>
+      <c r="B347" t="n">
+        <v>18.19968092068358</v>
+      </c>
+      <c r="C347" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>39.18424713352256</v>
+      </c>
+      <c r="B348" t="n">
+        <v>21.34444400402432</v>
+      </c>
+      <c r="C348" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>35.50229885420853</v>
+      </c>
+      <c r="B349" t="n">
+        <v>16.10401623198925</v>
+      </c>
+      <c r="C349" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>45.48850970305306</v>
+      </c>
+      <c r="B350" t="n">
+        <v>15.59301156712013</v>
+      </c>
+      <c r="C350" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>28.88859700647797</v>
+      </c>
+      <c r="B351" t="n">
+        <v>9.837045818009035</v>
+      </c>
+      <c r="C351" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>14.78376983753207</v>
+      </c>
+      <c r="B352" t="n">
+        <v>6.862055356117985</v>
+      </c>
+      <c r="C352" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>38.5297914889198</v>
+      </c>
+      <c r="B353" t="n">
+        <v>22.94431515906653</v>
+      </c>
+      <c r="C353" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>40.4314019446759</v>
+      </c>
+      <c r="B354" t="n">
+        <v>23.00836114326661</v>
+      </c>
+      <c r="C354" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>32.45108790277985</v>
+      </c>
+      <c r="B355" t="n">
+        <v>17.66202914546536</v>
+      </c>
+      <c r="C355" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>40.83868719818244</v>
+      </c>
+      <c r="B356" t="n">
+        <v>11.78059582097401</v>
+      </c>
+      <c r="C356" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>29.75182385457563</v>
+      </c>
+      <c r="B357" t="n">
+        <v>11.98419149225322</v>
+      </c>
+      <c r="C357" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>27.10164073434198</v>
+      </c>
+      <c r="B358" t="n">
+        <v>22.94220519905154</v>
+      </c>
+      <c r="C358" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>11.01676506976381</v>
+      </c>
+      <c r="B359" t="n">
+        <v>22.74172848530235</v>
+      </c>
+      <c r="C359" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>14.31565707973218</v>
+      </c>
+      <c r="B360" t="n">
+        <v>20.59751091715248</v>
+      </c>
+      <c r="C360" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>